<commit_message>
adding zoom value for google map default zooming scale when display company location
</commit_message>
<xml_diff>
--- a/data/development/userData/catalog.xlsx
+++ b/data/development/userData/catalog.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CCF8A5-0534-48CB-9406-F555059DEB5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605A154C-2343-4C89-BA7F-7E5326282578}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="4" xr2:uid="{7793E359-B97B-41D0-B964-1A54AF17E755}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" xr2:uid="{7793E359-B97B-41D0-B964-1A54AF17E755}"/>
   </bookViews>
   <sheets>
     <sheet name="categories" sheetId="170" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="generalSpecs" sheetId="179" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">categories!$A$1:$B$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">categories!$A$1:$B$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">features!$A$1:$C$510</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">photos!$A$1:$F$892</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">products!$A$1:$E$165</definedName>
@@ -10803,8 +10803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10823,101 +10823,104 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2007</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2006</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1999</v>
+        <v>1994</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1993</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1593</v>
+        <v>1995</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1993</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1997</v>
-      </c>
-      <c r="B5" t="s">
         <v>1996</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2006</v>
+        <v>1997</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1996</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1993</v>
+        <v>1998</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1996</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2005</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2003</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2004</v>
+        <v>2000</v>
       </c>
       <c r="B9" t="s">
-        <v>2003</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1995</v>
+        <v>2001</v>
       </c>
       <c r="B10" t="s">
-        <v>1993</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2010</v>
+        <v>2002</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1999</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1998</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1996</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>2009</v>
+        <v>2004</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2003</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>2001</v>
+        <v>2005</v>
       </c>
       <c r="B14" t="s">
-        <v>1999</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>2000</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1999</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="B16" t="s">
         <v>2006</v>
@@ -10925,28 +10928,25 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>2002</v>
+        <v>2008</v>
       </c>
       <c r="B17" t="s">
-        <v>1999</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1994</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1993</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>2003</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1996</v>
+        <v>2010</v>
       </c>
     </row>
   </sheetData>
@@ -19556,7 +19556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD3F4349-1EB2-4F66-BEAE-FA963E498509}">
   <dimension ref="A1:F892"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
category sorting functionality implemented
</commit_message>
<xml_diff>
--- a/data/development/userData/catalog.xlsx
+++ b/data/development/userData/catalog.xlsx
@@ -3,10 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE343151-1D40-46C2-89B3-97A7AE4E3A43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A11208-F3EB-4270-8967-EEA431A8E316}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="4" xr2:uid="{7793E359-B97B-41D0-B964-1A54AF17E755}"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25485" windowHeight="8055" activeTab="1" xr2:uid="{F6190CDE-D8DD-4F22-964B-351ACE1680E5}"/>
   </bookViews>
   <sheets>
     <sheet name="categories" sheetId="170" r:id="rId1"/>
@@ -10965,9 +10964,6 @@
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="A20" sqref="A20"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11123,7 +11119,6 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11174,7 +11169,6 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11287,7 +11281,6 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11358,9 +11351,6 @@
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="1">
-      <selection activeCell="A47" sqref="A47"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11758,9 +11748,6 @@
     <sheetView topLeftCell="B112" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
-    <sheetView topLeftCell="A145" workbookViewId="1">
-      <selection activeCell="B165" sqref="B165"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14098,7 +14085,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19731,7 +19717,6 @@
     <sheetView tabSelected="1" topLeftCell="A295" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D90" sqref="D90"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -33485,7 +33470,6 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -33528,7 +33512,6 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -33588,7 +33571,6 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -33784,7 +33766,6 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>